<commit_message>
Use id linea agg to trear different branches as one line
</commit_message>
<xml_diff>
--- a/docs/configuraciones.xlsx
+++ b/docs/configuraciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sanapolsky\Google Drive\Python 2.0\github\UrbanTrips\UrbanTrips\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED84857-E966-49FB-A386-F357A2D36FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21BFB56-4101-4838-8A1D-2EE5CEB8B105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="146">
   <si>
     <t>variable</t>
   </si>
@@ -320,9 +320,6 @@
     <t>trxs</t>
   </si>
   <si>
-    <t>especifica si ordena transacciones por fecha o por variable orden_trx</t>
-  </si>
-  <si>
     <t>ventana de tiempo para que una transacción sea de un mismo viaje (ej. 60 minutos)</t>
   </si>
   <si>
@@ -468,6 +465,12 @@
   </si>
   <si>
     <t>Valor de la variable que marca el fin del servicio</t>
+  </si>
+  <si>
+    <t>especifica si ordena transacciones por fecha ("fecha_completa") o por variable orden_trx ("orden_trx") en la tabla nombres_variables_trx</t>
+  </si>
+  <si>
+    <t>Archivo .csv con lineas, debe contener ("id_linea", "nombre_linea", "modo")</t>
   </si>
 </sst>
 </file>
@@ -864,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,16 +889,16 @@
         <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>55</v>
@@ -904,10 +907,10 @@
         <v>59</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>90</v>
@@ -1212,10 +1215,10 @@
         <v>60</v>
       </c>
       <c r="H17" t="s">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="I17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1232,7 +1235,7 @@
         <v>120</v>
       </c>
       <c r="H18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1249,7 +1252,7 @@
         <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1257,7 +1260,7 @@
         <v>2.44</v>
       </c>
       <c r="B20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
@@ -1269,7 +1272,7 @@
         <v>93</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1277,7 +1280,7 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
@@ -1289,10 +1292,10 @@
         <v>60</v>
       </c>
       <c r="H21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1300,7 +1303,7 @@
         <v>2.46</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -1312,7 +1315,7 @@
         <v>60</v>
       </c>
       <c r="H22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1320,7 +1323,7 @@
         <v>2.5</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -1332,10 +1335,10 @@
         <v>60</v>
       </c>
       <c r="H23" t="s">
+        <v>115</v>
+      </c>
+      <c r="I23" t="s">
         <v>116</v>
-      </c>
-      <c r="I23" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1343,7 +1346,7 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -1355,7 +1358,7 @@
         <v>60</v>
       </c>
       <c r="H24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1372,7 +1375,7 @@
         <v>52</v>
       </c>
       <c r="H25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>72</v>
@@ -1389,7 +1392,7 @@
         <v>16</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1397,13 +1400,13 @@
         <v>2.7</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G27" t="s">
         <v>60</v>
@@ -1414,13 +1417,13 @@
         <v>2.71</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" t="s">
         <v>62</v>
       </c>
       <c r="H28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1428,7 +1431,7 @@
         <v>2.8</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
         <v>63</v>
@@ -1437,7 +1440,7 @@
         <v>64</v>
       </c>
       <c r="I29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1445,7 +1448,7 @@
         <v>2.81</v>
       </c>
       <c r="B30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C30" t="s">
         <v>63</v>
@@ -1459,7 +1462,7 @@
         <v>2.82</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
         <v>63</v>
@@ -1473,7 +1476,7 @@
         <v>2.83</v>
       </c>
       <c r="B32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
         <v>63</v>
@@ -1487,7 +1490,7 @@
         <v>2.84</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
         <v>63</v>
@@ -1501,7 +1504,7 @@
         <v>2.85</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
         <v>63</v>
@@ -1515,7 +1518,7 @@
         <v>2.86</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
         <v>63</v>
@@ -1529,13 +1532,13 @@
         <v>2.87</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36" t="s">
         <v>63</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E36" t="s">
         <v>60</v>
@@ -1546,13 +1549,13 @@
         <v>2.88</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C37" t="s">
         <v>63</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1560,16 +1563,16 @@
         <v>2.89</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J38" s="3"/>
     </row>
@@ -1578,13 +1581,19 @@
         <v>2.9</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
         <v>61</v>
       </c>
+      <c r="G39" t="s">
+        <v>60</v>
+      </c>
+      <c r="H39" t="s">
+        <v>145</v>
+      </c>
       <c r="I39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -1592,7 +1601,7 @@
         <v>2.91</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -1603,7 +1612,7 @@
         <v>2.92</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
@@ -1615,10 +1624,10 @@
         <v>60</v>
       </c>
       <c r="H41" t="s">
+        <v>129</v>
+      </c>
+      <c r="J41" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1626,10 +1635,10 @@
         <v>2.93</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J42" s="3"/>
     </row>
@@ -1638,23 +1647,23 @@
         <v>2.94</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C43" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D43" s="4"/>
       <c r="F43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G43" t="s">
         <v>60</v>
       </c>
       <c r="H43" t="s">
+        <v>139</v>
+      </c>
+      <c r="I43" t="s">
         <v>140</v>
-      </c>
-      <c r="I43" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -1662,13 +1671,13 @@
         <v>2.95</v>
       </c>
       <c r="B44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="H44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J44" s="3"/>
     </row>
@@ -1677,13 +1686,13 @@
         <v>2.96</v>
       </c>
       <c r="B45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J45" s="3"/>
     </row>
@@ -1773,7 +1782,7 @@
         <v>5.2</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C52" t="s">
         <v>14</v>
@@ -1787,7 +1796,7 @@
         <v>5.3</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C53" t="s">
         <v>14</v>
@@ -1801,7 +1810,7 @@
         <v>5.4</v>
       </c>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
@@ -1815,7 +1824,7 @@
         <v>5.5</v>
       </c>
       <c r="B55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
@@ -1838,7 +1847,7 @@
         <v>43</v>
       </c>
       <c r="I56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -1964,7 +1973,7 @@
         <v>21</v>
       </c>
       <c r="D65" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1978,7 +1987,7 @@
         <v>21</v>
       </c>
       <c r="D66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1992,7 +2001,7 @@
         <v>21</v>
       </c>
       <c r="D67" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2006,7 +2015,7 @@
         <v>21</v>
       </c>
       <c r="D68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2020,7 +2029,7 @@
         <v>21</v>
       </c>
       <c r="D69" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2034,7 +2043,7 @@
         <v>21</v>
       </c>
       <c r="D70" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Indicadores de oferta y demanda en dash
</commit_message>
<xml_diff>
--- a/docs/configuraciones.xlsx
+++ b/docs/configuraciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sanapolsky\Google Drive\Python 2.0\github\UrbanTrips\UrbanTrips\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0F1396-5338-4D6C-9616-F04A3E8BF42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8645DDE4-2D88-40F4-BEFD-98BCE91D35E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="148">
   <si>
     <t>variable</t>
   </si>
@@ -874,7 +874,7 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,9 +1160,6 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="G14" t="s">
-        <v>59</v>
-      </c>
       <c r="H14" t="s">
         <v>85</v>
       </c>
@@ -1179,9 +1176,6 @@
       </c>
       <c r="D15" t="s">
         <v>31</v>
-      </c>
-      <c r="G15" t="s">
-        <v>59</v>
       </c>
       <c r="H15" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
classify legs into stations in process transaccions and legs module
</commit_message>
<xml_diff>
--- a/docs/configuraciones.xlsx
+++ b/docs/configuraciones.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="153">
   <si>
     <t xml:space="preserve">orden</t>
   </si>
@@ -688,11 +688,11 @@
   </sheetPr>
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C71" activeCellId="0" sqref="C71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G71" activeCellId="0" sqref="G71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
@@ -1889,9 +1889,6 @@
       <c r="C71" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="G71" s="0" t="s">
-        <v>83</v>
-      </c>
       <c r="H71" s="0" t="s">
         <v>152</v>
       </c>

</xml_diff>

<commit_message>
Adds new modes (#165)
- Adds new modes 
- Adds db_alias_dashboard

---------

Co-authored-by: Sebastian Anapolsky <sanapolsky@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/configuraciones.xlsx
+++ b/docs/configuraciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sanapolsky\Google Drive\Python 2.0\github\UrbanTrips\UrbanTrips\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622CB803-6D12-4EED-BA7E-14BF73CFE082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8229F57E-8491-46EB-898E-32E497E2A5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="163">
   <si>
     <t>orden</t>
   </si>
@@ -496,6 +496,24 @@
   </si>
   <si>
     <t>Indica el tipo de tarifa asignado a la transacción</t>
+  </si>
+  <si>
+    <t>cable</t>
+  </si>
+  <si>
+    <t>otros</t>
+  </si>
+  <si>
+    <t>lancha</t>
+  </si>
+  <si>
+    <t>alias_db_dashboard</t>
+  </si>
+  <si>
+    <t>db_dash</t>
+  </si>
+  <si>
+    <t>nombre del sqlite donde se guardan los datos a mostrar en el dashboard</t>
   </si>
 </sst>
 </file>
@@ -983,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,27 +1113,27 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2.0099999999999998</v>
+        <v>1.4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
+        <v>160</v>
+      </c>
+      <c r="F5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>25</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>2.02</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -1124,18 +1142,18 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>2.0299999999999998</v>
+        <v>2.02</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -1144,18 +1162,18 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>2.04</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -1164,15 +1182,18 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>2.0499999999999998</v>
+        <v>2.04</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
@@ -1181,15 +1202,15 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>2.06</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
@@ -1198,18 +1219,15 @@
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2.0699999999999998</v>
+        <v>2.06</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
@@ -1218,15 +1236,18 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>2.08</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
@@ -1235,15 +1256,15 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>2.09</v>
+        <v>2.08</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
@@ -1252,15 +1273,15 @@
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2.1</v>
+        <v>2.09</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -1269,15 +1290,15 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>153</v>
+        <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>155</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>2.11</v>
+        <v>2.1</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
@@ -1286,15 +1307,15 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>2.12</v>
+        <v>2.11</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
@@ -1303,15 +1324,15 @@
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>154</v>
       </c>
       <c r="H16" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>2.13</v>
+        <v>2.12</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
@@ -1320,15 +1341,15 @@
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>2.14</v>
+        <v>2.13</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
@@ -1337,263 +1358,263 @@
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>2.21</v>
+        <v>2.14</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
       </c>
       <c r="H19" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>2.2200000000000002</v>
+        <v>2.21</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20">
-        <v>120</v>
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="I20" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>2.23</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="B21" t="s">
         <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="H21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>2.44</v>
+        <v>2.23</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" t="s">
-        <v>12</v>
+        <v>55</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
       </c>
       <c r="H22" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" t="s">
-        <v>60</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>2.4500000000000002</v>
+        <v>2.44</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23">
-        <v>2000</v>
-      </c>
-      <c r="G23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" t="s">
         <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I23" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>2.46</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="B24" t="s">
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" t="s">
-        <v>12</v>
+        <v>63</v>
+      </c>
+      <c r="F24">
+        <v>2000</v>
       </c>
       <c r="G24" t="s">
         <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="I24" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>2.5</v>
+        <v>2.46</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25">
-        <v>8</v>
+        <v>66</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>70</v>
-      </c>
-      <c r="I25" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>2.5099999999999998</v>
+        <v>2.5</v>
       </c>
       <c r="B26" t="s">
         <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F26">
-        <v>9265</v>
+        <v>8</v>
       </c>
       <c r="G26" t="s">
         <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="I26" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>2.6</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="F27">
+        <v>9265</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>77</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>2.61</v>
+        <v>2.6</v>
       </c>
       <c r="B28" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>79</v>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" t="s">
+        <v>77</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>2.7</v>
+        <v>2.61</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" t="s">
-        <v>82</v>
-      </c>
-      <c r="F29" t="s">
-        <v>83</v>
-      </c>
-      <c r="G29" t="s">
-        <v>12</v>
+        <v>74</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>2.71</v>
+        <v>2.7</v>
       </c>
       <c r="B30" t="s">
         <v>81</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
-      </c>
-      <c r="H30" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="F30" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>2.8</v>
+        <v>2.71</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" t="s">
-        <v>88</v>
-      </c>
-      <c r="I31" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="H31" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>2.81</v>
+        <v>2.8</v>
       </c>
       <c r="B32" t="s">
         <v>86</v>
@@ -1602,12 +1623,15 @@
         <v>87</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="I32" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>2.82</v>
+        <v>2.81</v>
       </c>
       <c r="B33" t="s">
         <v>86</v>
@@ -1616,12 +1640,12 @@
         <v>87</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>2.83</v>
+        <v>2.82</v>
       </c>
       <c r="B34" t="s">
         <v>86</v>
@@ -1630,12 +1654,12 @@
         <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>2.84</v>
+        <v>2.83</v>
       </c>
       <c r="B35" t="s">
         <v>86</v>
@@ -1644,12 +1668,12 @@
         <v>87</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>2.85</v>
+        <v>2.84</v>
       </c>
       <c r="B36" t="s">
         <v>86</v>
@@ -1658,12 +1682,12 @@
         <v>87</v>
       </c>
       <c r="D36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>2.86</v>
+        <v>2.85</v>
       </c>
       <c r="B37" t="s">
         <v>86</v>
@@ -1672,12 +1696,12 @@
         <v>87</v>
       </c>
       <c r="D37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>2.88</v>
+        <v>2.86</v>
       </c>
       <c r="B38" t="s">
         <v>86</v>
@@ -1685,175 +1709,175 @@
       <c r="C38" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>96</v>
+      <c r="D38" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>2.89</v>
+        <v>2.88</v>
       </c>
       <c r="B39" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" t="s">
         <v>87</v>
       </c>
-      <c r="D39" t="s">
-        <v>97</v>
-      </c>
-      <c r="H39" t="s">
-        <v>98</v>
-      </c>
-      <c r="J39" s="4"/>
+      <c r="D39" s="3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>2.9</v>
+        <v>2.89</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" t="s">
-        <v>100</v>
-      </c>
-      <c r="G40" t="s">
-        <v>12</v>
+        <v>86</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" t="s">
+        <v>97</v>
       </c>
       <c r="H40" t="s">
-        <v>101</v>
-      </c>
-      <c r="I40" t="s">
-        <v>102</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="J40" s="4"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>2.92</v>
+        <v>2.9</v>
       </c>
       <c r="B41" t="s">
         <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
-      </c>
-      <c r="F41" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="G41" t="s">
         <v>12</v>
       </c>
       <c r="H41" t="s">
-        <v>104</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
+      </c>
+      <c r="I41" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>2.93</v>
+        <v>2.92</v>
       </c>
       <c r="B42" t="s">
         <v>99</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="J42" s="4"/>
+      <c r="C42" t="s">
+        <v>103</v>
+      </c>
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" t="s">
+        <v>12</v>
+      </c>
+      <c r="H42" t="s">
+        <v>104</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>2.931</v>
+        <v>2.93</v>
       </c>
       <c r="B43" t="s">
         <v>99</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F43">
-        <v>5</v>
-      </c>
-      <c r="G43" t="s">
-        <v>12</v>
-      </c>
-      <c r="H43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J43" s="4"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>2.94</v>
+        <v>2.931</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" t="s">
-        <v>109</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="F44" t="s">
-        <v>83</v>
+        <v>99</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F44">
+        <v>5</v>
       </c>
       <c r="G44" t="s">
         <v>12</v>
       </c>
       <c r="H44" t="s">
-        <v>110</v>
-      </c>
-      <c r="I44" t="s">
-        <v>111</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>2.95</v>
+        <v>2.94</v>
       </c>
       <c r="B45" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>112</v>
+      <c r="C45" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="F45" t="s">
+        <v>83</v>
+      </c>
+      <c r="G45" t="s">
+        <v>12</v>
       </c>
       <c r="H45" t="s">
-        <v>113</v>
-      </c>
-      <c r="J45" s="4"/>
+        <v>110</v>
+      </c>
+      <c r="I45" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>2.96</v>
+        <v>2.95</v>
       </c>
       <c r="B46" t="s">
         <v>97</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J46" s="4"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>4.0999999999999996</v>
+        <v>2.96</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
-      </c>
-      <c r="C47" t="s">
-        <v>116</v>
-      </c>
-      <c r="D47" t="s">
-        <v>117</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H47" t="s">
+        <v>115</v>
+      </c>
+      <c r="J47" s="4"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B48" t="s">
         <v>116</v>
@@ -1862,12 +1886,12 @@
         <v>116</v>
       </c>
       <c r="D48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="B49" t="s">
         <v>116</v>
@@ -1876,12 +1900,12 @@
         <v>116</v>
       </c>
       <c r="D49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="B50" t="s">
         <v>116</v>
@@ -1890,12 +1914,12 @@
         <v>116</v>
       </c>
       <c r="D50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>4.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B51" t="s">
         <v>116</v>
@@ -1904,144 +1928,141 @@
         <v>116</v>
       </c>
       <c r="D51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>5.0999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="B52" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C52" t="s">
-        <v>123</v>
-      </c>
-      <c r="H52" t="s">
-        <v>124</v>
-      </c>
-      <c r="I52" t="s">
-        <v>125</v>
+        <v>116</v>
+      </c>
+      <c r="D52" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>5.2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C53" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D53" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>5.3</v>
+        <v>4.7</v>
       </c>
       <c r="B54" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D54" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="B55" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C55" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D55" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>5.5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B56" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C56" t="s">
-        <v>127</v>
-      </c>
-      <c r="D56" t="s">
-        <v>131</v>
+        <v>123</v>
+      </c>
+      <c r="H56" t="s">
+        <v>124</v>
+      </c>
+      <c r="I56" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>6.1</v>
+        <v>5.2</v>
       </c>
       <c r="B57" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C57" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D57" t="s">
-        <v>133</v>
-      </c>
-      <c r="I57" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>6.2</v>
+        <v>5.3</v>
       </c>
       <c r="B58" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C58" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D58" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>6.3</v>
+        <v>5.4</v>
       </c>
       <c r="B59" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C59" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D59" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
       <c r="B60" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C60" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D60" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>6.5</v>
+        <v>6.1</v>
       </c>
       <c r="B61" t="s">
         <v>132</v>
@@ -2050,12 +2071,15 @@
         <v>132</v>
       </c>
       <c r="D61" t="s">
-        <v>138</v>
+        <v>133</v>
+      </c>
+      <c r="I61" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="B62" t="s">
         <v>132</v>
@@ -2064,12 +2088,12 @@
         <v>132</v>
       </c>
       <c r="D62" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>6.7</v>
+        <v>6.3</v>
       </c>
       <c r="B63" t="s">
         <v>132</v>
@@ -2078,12 +2102,12 @@
         <v>132</v>
       </c>
       <c r="D63" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>6.8</v>
+        <v>6.4</v>
       </c>
       <c r="B64" t="s">
         <v>132</v>
@@ -2092,12 +2116,12 @@
         <v>132</v>
       </c>
       <c r="D64" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>6.9</v>
+        <v>6.5</v>
       </c>
       <c r="B65" t="s">
         <v>132</v>
@@ -2106,12 +2130,12 @@
         <v>132</v>
       </c>
       <c r="D65" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>7</v>
+        <v>6.6</v>
       </c>
       <c r="B66" t="s">
         <v>132</v>
@@ -2120,12 +2144,12 @@
         <v>132</v>
       </c>
       <c r="D66" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>7.1</v>
+        <v>6.7</v>
       </c>
       <c r="B67" t="s">
         <v>132</v>
@@ -2134,12 +2158,12 @@
         <v>132</v>
       </c>
       <c r="D67" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>7.2</v>
+        <v>6.8</v>
       </c>
       <c r="B68" t="s">
         <v>132</v>
@@ -2148,12 +2172,12 @@
         <v>132</v>
       </c>
       <c r="D68" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>7.3</v>
+        <v>6.9</v>
       </c>
       <c r="B69" t="s">
         <v>132</v>
@@ -2162,12 +2186,12 @@
         <v>132</v>
       </c>
       <c r="D69" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>7.4</v>
+        <v>7</v>
       </c>
       <c r="B70" t="s">
         <v>132</v>
@@ -2176,12 +2200,12 @@
         <v>132</v>
       </c>
       <c r="D70" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>7.5</v>
+        <v>7.1</v>
       </c>
       <c r="B71" t="s">
         <v>132</v>
@@ -2190,37 +2214,93 @@
         <v>132</v>
       </c>
       <c r="D71" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>8.1</v>
+        <v>7.2</v>
       </c>
       <c r="B72" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="C72" t="s">
-        <v>149</v>
-      </c>
-      <c r="G72" t="s">
-        <v>83</v>
-      </c>
-      <c r="H72" t="s">
-        <v>150</v>
+        <v>132</v>
+      </c>
+      <c r="D72" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B73" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73" t="s">
+        <v>132</v>
+      </c>
+      <c r="D73" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="B74" t="s">
+        <v>132</v>
+      </c>
+      <c r="C74" t="s">
+        <v>132</v>
+      </c>
+      <c r="D74" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="B75" t="s">
+        <v>132</v>
+      </c>
+      <c r="C75" t="s">
+        <v>132</v>
+      </c>
+      <c r="D75" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="B76" t="s">
+        <v>149</v>
+      </c>
+      <c r="C76" t="s">
+        <v>149</v>
+      </c>
+      <c r="G76" t="s">
+        <v>83</v>
+      </c>
+      <c r="H76" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
         <v>9.1</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B77" t="s">
         <v>151</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C77" t="s">
         <v>151</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H77" t="s">
         <v>152</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corridas multiples en dash
</commit_message>
<xml_diff>
--- a/docs/configuraciones.xlsx
+++ b/docs/configuraciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sanapolsky\Google Drive\Python 2.0\github\UrbanTrips\UrbanTrips\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEF11E7-1C69-4264-B717-99442E0CC0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36563865-838A-449E-A114-AAE526FDAAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="168">
   <si>
     <t>orden</t>
   </si>
@@ -517,6 +517,18 @@
   </si>
   <si>
     <t>distance_gps</t>
+  </si>
+  <si>
+    <t>dash_configs</t>
+  </si>
+  <si>
+    <t>alias_dash_lista</t>
+  </si>
+  <si>
+    <t>alias_data_lista</t>
+  </si>
+  <si>
+    <t>alias_insumos_lista</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,7 +2333,52 @@
         <v>152</v>
       </c>
     </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="B79" t="s">
+        <v>164</v>
+      </c>
+      <c r="C79" t="s">
+        <v>164</v>
+      </c>
+      <c r="D79" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C80" t="s">
+        <v>164</v>
+      </c>
+      <c r="D80" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>10.3</v>
+      </c>
+      <c r="B81" t="s">
+        <v>164</v>
+      </c>
+      <c r="C81" t="s">
+        <v>164</v>
+      </c>
+      <c r="D81" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J78">
+    <sortCondition ref="A2:A78"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Multiple alias in dashboard (#200)
* corridas multiples en dash

---------

Co-authored-by: Sebastian Anapolsky <sanapolsky@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/configuraciones.xlsx
+++ b/docs/configuraciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sanapolsky\Google Drive\Python 2.0\github\UrbanTrips\UrbanTrips\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEF11E7-1C69-4264-B717-99442E0CC0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36563865-838A-449E-A114-AAE526FDAAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="168">
   <si>
     <t>orden</t>
   </si>
@@ -517,6 +517,18 @@
   </si>
   <si>
     <t>distance_gps</t>
+  </si>
+  <si>
+    <t>dash_configs</t>
+  </si>
+  <si>
+    <t>alias_dash_lista</t>
+  </si>
+  <si>
+    <t>alias_data_lista</t>
+  </si>
+  <si>
+    <t>alias_insumos_lista</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,7 +2333,52 @@
         <v>152</v>
       </c>
     </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="B79" t="s">
+        <v>164</v>
+      </c>
+      <c r="C79" t="s">
+        <v>164</v>
+      </c>
+      <c r="D79" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C80" t="s">
+        <v>164</v>
+      </c>
+      <c r="D80" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>10.3</v>
+      </c>
+      <c r="B81" t="s">
+        <v>164</v>
+      </c>
+      <c r="C81" t="s">
+        <v>164</v>
+      </c>
+      <c r="D81" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J78">
+    <sortCondition ref="A2:A78"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Update h3 librarty to api v4
</commit_message>
<xml_diff>
--- a/docs/configuraciones.xlsx
+++ b/docs/configuraciones.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">True</t>
   </si>
   <si>
-    <t xml:space="preserve">Listar los nombres de las corridas [‘lunes’,’martes’], deben coincidir con los archivos trx y gps,por ej lunes_trx.csv, lunes_gps.csv, martes_trx.csv, martes_gps.csv</t>
+    <t xml:space="preserve">Listar los nombres de las corridas [“lunes”,”martes”], deben coincidir con los archivos trx y gps,por ej lunes_trx.csv, lunes_gps.csv, martes_trx.csv, martes_gps.csv</t>
   </si>
   <si>
     <t xml:space="preserve">archivo_transacciones</t>
@@ -880,8 +880,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>